<commit_message>
Documentation & Town Update
</commit_message>
<xml_diff>
--- a/Documentation/Objectives, Achievements, etc./Achievements Breakdown.xlsx
+++ b/Documentation/Objectives, Achievements, etc./Achievements Breakdown.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -172,6 +172,15 @@
   </si>
   <si>
     <t>Main Demon</t>
+  </si>
+  <si>
+    <t>This Game is Home Grown</t>
+  </si>
+  <si>
+    <t>Found all collectables</t>
+  </si>
+  <si>
+    <t>Saskatchewan Shaped, but spooky</t>
   </si>
 </sst>
 </file>
@@ -249,8 +258,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -288,7 +299,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -298,6 +309,7 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -307,6 +319,7 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -638,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -746,7 +759,9 @@
       <c r="B7" s="1">
         <v>4</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4" t="s">
         <v>12</v>
@@ -931,12 +946,18 @@
       <c r="B18" s="1">
         <v>15</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="C18" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="E18" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="4"/>
+      <c r="F18" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="G18" s="4" t="s">
         <v>29</v>
       </c>

</xml_diff>